<commit_message>
ACID weapon without checked Balanced damage Trace and hits images
</commit_message>
<xml_diff>
--- a/Descriptions/Shooting.xlsx
+++ b/Descriptions/Shooting.xlsx
@@ -435,7 +435,7 @@
   </si>
   <si>
     <r>
-      <t>66</t>
+      <t>62</t>
     </r>
     <r>
       <rPr>
@@ -450,7 +450,7 @@
   </si>
   <si>
     <r>
-      <t>72</t>
+      <t>80</t>
     </r>
     <r>
       <rPr>
@@ -465,105 +465,276 @@
   </si>
   <si>
     <r>
+      <t>42</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFEEEEEE"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|44</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>48</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFEEEEEE"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|42</t>
+    </r>
+  </si>
+  <si>
+    <t>STR_ROCKET_LAUNCHER</t>
+  </si>
+  <si>
+    <r>
+      <t>55</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|55</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|115</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>45</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|45</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>75</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|75</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>120</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFEEEEEE"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|100</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>140</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFEEEEEE"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|90</t>
+    </r>
+  </si>
+  <si>
+    <t>STR_LASER_PISTOL</t>
+  </si>
+  <si>
+    <r>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|28</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|40</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>68</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|68</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|25</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|20</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>33</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|55</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>40</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FFEEEEEE"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|44</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>48</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFEEEEEE"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|42</t>
-    </r>
-  </si>
-  <si>
-    <t>STR_ROCKET_LAUNCHER</t>
-  </si>
-  <si>
-    <r>
-      <t>55</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|55</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|115</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>45</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|45</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>75</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|75</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>100</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFEEEEEE"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|46</t>
+    </r>
+  </si>
+  <si>
+    <t>STR_LASER_RIFLE</t>
+  </si>
+  <si>
+    <r>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|46</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>60</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|65</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>85</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
@@ -573,24 +744,6 @@
   </si>
   <si>
     <r>
-      <t>125</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFEEEEEE"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|90</t>
-    </r>
-  </si>
-  <si>
-    <t>STR_LASER_PISTOL</t>
-  </si>
-  <si>
-    <r>
       <t>0</t>
     </r>
     <r>
@@ -601,22 +754,22 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>|28</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>50</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|40</t>
+      <t>|34</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>24</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|25</t>
     </r>
   </si>
   <si>
@@ -631,165 +784,12 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>|68</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|25</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|20</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>33</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|55</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>42</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFDDDDDD"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|46</t>
-    </r>
-  </si>
-  <si>
-    <t>STR_LASER_RIFLE</t>
-  </si>
-  <si>
-    <r>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|46</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>60</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|65</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>85</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|100</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|34</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>24</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>|25</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>68</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFCCCCCC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
       <t>|50</t>
     </r>
   </si>
   <si>
     <r>
-      <t>55</t>
+      <t>56</t>
     </r>
     <r>
       <rPr>
@@ -1398,7 +1398,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1480,7 +1480,7 @@
         <v>16</v>
       </c>
       <c r="I2" s="8" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J2" s="4" t="n">
         <v>5</v>
@@ -1526,7 +1526,7 @@
         <v>26</v>
       </c>
       <c r="I3" s="8" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J3" s="4" t="n">
         <v>5</v>
@@ -1576,7 +1576,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="8" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J4" s="9" t="n">
         <v>2</v>
@@ -1622,7 +1622,7 @@
         <v>40</v>
       </c>
       <c r="I5" s="13" t="n">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J5" s="12" t="n">
         <v>3</v>
@@ -1670,7 +1670,7 @@
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="8" t="n">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J6" s="4" t="n">
         <v>2</v>
@@ -1706,7 +1706,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="17" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="17" t="n">
@@ -1770,7 +1770,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="4" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P8" s="10" t="s">
         <v>28</v>
@@ -1953,10 +1953,10 @@
         <v>66</v>
       </c>
       <c r="H13" s="21" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="I13" s="22" t="n">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="J13" s="4" t="n">
         <v>3</v>
@@ -2374,7 +2374,7 @@
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="17" t="n">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H22" s="12" t="n">
         <v>120</v>

</xml_diff>

<commit_message>
research of alien's weapons was corrected for much more dependencies
</commit_message>
<xml_diff>
--- a/Descriptions/Shooting.xlsx
+++ b/Descriptions/Shooting.xlsx
@@ -1383,7 +1383,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1686,12 +1686,12 @@
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="17" t="n">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="17" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="17" t="n">
@@ -2359,10 +2359,10 @@
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="17" t="n">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="H22" s="12" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="I22" s="26"/>
       <c r="J22" s="12" t="n">

</xml_diff>

<commit_message>
Rail gun improve images Balance plasma and sniper rifles Balance laser weapons
</commit_message>
<xml_diff>
--- a/Descriptions/Shooting.xlsx
+++ b/Descriptions/Shooting.xlsx
@@ -1378,8 +1378,8 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1566,7 +1566,7 @@
         <v>2</v>
       </c>
       <c r="L4" s="9" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M4" s="9" t="n">
         <v>20</v>
@@ -1594,7 +1594,7 @@
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" s="13" t="n">
         <v>80</v>
@@ -1687,7 +1687,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="17" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="17" t="n">
@@ -2232,16 +2232,16 @@
         <v>1</v>
       </c>
       <c r="L19" s="4" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="M19" s="4" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N19" s="4" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="O19" s="4" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="P19" s="10" t="s">
         <v>78</v>
@@ -2280,16 +2280,16 @@
         <v>2</v>
       </c>
       <c r="L20" s="4" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="M20" s="4" t="n">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N20" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O20" s="4" t="n">
         <v>50</v>
-      </c>
-      <c r="O20" s="4" t="n">
-        <v>65</v>
       </c>
       <c r="P20" s="10" t="s">
         <v>86</v>
@@ -2328,16 +2328,16 @@
         <v>3</v>
       </c>
       <c r="L21" s="12" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M21" s="12" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="N21" s="12" t="n">
+        <v>40</v>
+      </c>
+      <c r="O21" s="12" t="n">
         <v>50</v>
-      </c>
-      <c r="O21" s="12" t="n">
-        <v>65</v>
       </c>
       <c r="P21" s="15" t="s">
         <v>91</v>
@@ -2355,7 +2355,7 @@
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="17" t="n">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="17" t="n">
@@ -2374,10 +2374,10 @@
         <v>0</v>
       </c>
       <c r="N22" s="12" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="O22" s="12" t="n">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="P22" s="15" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
HEAVY LASER a litle bit much decrease damage
</commit_message>
<xml_diff>
--- a/Descriptions/Shooting.xlsx
+++ b/Descriptions/Shooting.xlsx
@@ -422,7 +422,19 @@
     </r>
   </si>
   <si>
-    <t>70X3</t>
+    <r>
+      <t>68X3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>|85</t>
+    </r>
   </si>
   <si>
     <t>HE</t>
@@ -1378,8 +1390,8 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1881,13 +1893,13 @@
         <v>0</v>
       </c>
       <c r="M11" s="12" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N11" s="12" t="n">
         <v>0</v>
       </c>
       <c r="O11" s="12" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="P11" s="15" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
PISTOL damage was increased
</commit_message>
<xml_diff>
--- a/Descriptions/Shooting.xlsx
+++ b/Descriptions/Shooting.xlsx
@@ -1390,8 +1390,8 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1473,7 +1473,7 @@
         <v>16</v>
       </c>
       <c r="I2" s="8" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J2" s="4" t="n">
         <v>5</v>
@@ -1519,7 +1519,7 @@
         <v>26</v>
       </c>
       <c r="I3" s="8" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J3" s="4" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
UFOpedia was checked till PLASMA
</commit_message>
<xml_diff>
--- a/Descriptions/Shooting.xlsx
+++ b/Descriptions/Shooting.xlsx
@@ -363,7 +363,7 @@
   </si>
   <si>
     <r>
-      <t>75</t>
+      <t>68</t>
     </r>
     <r>
       <rPr>
@@ -1391,7 +1391,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Images from PISTOL till SNIPER RIFLE was improved
</commit_message>
<xml_diff>
--- a/Descriptions/Shooting.xlsx
+++ b/Descriptions/Shooting.xlsx
@@ -393,7 +393,7 @@
   </si>
   <si>
     <r>
-      <t>34</t>
+      <t>35</t>
     </r>
     <r>
       <rPr>
@@ -1391,7 +1391,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
HEAVY Laser damage decresed by 4
</commit_message>
<xml_diff>
--- a/Descriptions/Shooting.xlsx
+++ b/Descriptions/Shooting.xlsx
@@ -423,7 +423,7 @@
   </si>
   <si>
     <r>
-      <t>64X3</t>
+      <t>60X3</t>
     </r>
     <r>
       <rPr>
@@ -1390,8 +1390,8 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>